<commit_message>
Integrated the new SciCharts into FDA coordinates function editors.
Former-commit-id: 9f31464c35e38f7314f563de11fe47b1373903dc
</commit_message>
<xml_diff>
--- a/FunctionsTests/ExcelTesting/ExcelData/ComposeTestData.xlsx
+++ b/FunctionsTests/ExcelTesting/ExcelData/ComposeTestData.xlsx
@@ -548,7 +548,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="M4" s="1">
-        <x:v>43854.55625</x:v>
+        <x:v>43857.6430555556</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="M12" s="1">
-        <x:v>43854.55625</x:v>
+        <x:v>43857.6430555556</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="M18" s="4">
-        <x:v>43854.55625</x:v>
+        <x:v>43857.6430555556</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Untested changes to Coordinates and _ExtendedCoordinates properties... with effects on compose.
Former-commit-id: 94a8828ee353340d59caa633b30f937247079454
</commit_message>
<xml_diff>
--- a/FunctionsTests/ExcelTesting/ExcelData/ComposeTestData.xlsx
+++ b/FunctionsTests/ExcelTesting/ExcelData/ComposeTestData.xlsx
@@ -12757,7 +12757,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="M7" s="14">
-        <x:v>43938.6208333333</x:v>
+        <x:v>43950.6055555556</x:v>
       </x:c>
       <x:c r="N7" s="9" t="s"/>
     </x:row>
@@ -12930,7 +12930,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="M15" s="14">
-        <x:v>43938.6208333333</x:v>
+        <x:v>43950.6055555556</x:v>
       </x:c>
       <x:c r="N15" s="9" t="s"/>
     </x:row>
@@ -13051,7 +13051,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="M21" s="15">
-        <x:v>43938.6208333333</x:v>
+        <x:v>43950.6055555556</x:v>
       </x:c>
       <x:c r="N21" s="9" t="s"/>
     </x:row>
@@ -13173,7 +13173,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="M27" s="15">
-        <x:v>43938.6208333333</x:v>
+        <x:v>43950.6055555556</x:v>
       </x:c>
       <x:c r="N27" s="9" t="s"/>
     </x:row>

</xml_diff>